<commit_message>
ran results in newton
</commit_message>
<xml_diff>
--- a/results/gru/dilemma/confidence/0.1/percents/scores-10.xlsx
+++ b/results/gru/dilemma/confidence/0.1/percents/scores-10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="51">
   <si>
     <t>0.95-negative</t>
   </si>
@@ -43,127 +43,112 @@
     <t>name</t>
   </si>
   <si>
+    <t>illegal</t>
+  </si>
+  <si>
+    <t>drugs</t>
+  </si>
+  <si>
     <t>software</t>
   </si>
   <si>
-    <t>illegal</t>
-  </si>
-  <si>
-    <t>drugs</t>
-  </si>
-  <si>
     <t>edward</t>
   </si>
   <si>
+    <t>tu</t>
+  </si>
+  <si>
+    <t>customers</t>
+  </si>
+  <si>
     <t>two</t>
   </si>
   <si>
-    <t>tu</t>
-  </si>
-  <si>
-    <t>customers</t>
-  </si>
-  <si>
     <t>industries</t>
   </si>
   <si>
-    <t>refer</t>
-  </si>
-  <si>
-    <t>users</t>
-  </si>
-  <si>
     <t>:</t>
   </si>
   <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>th</t>
+  </si>
+  <si>
+    <t>are</t>
+  </si>
+  <si>
+    <t>only</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
     <t>that</t>
   </si>
   <si>
-    <t>—</t>
-  </si>
-  <si>
-    <t>th</t>
-  </si>
-  <si>
-    <t>only</t>
-  </si>
-  <si>
-    <t>there</t>
+    <t>.</t>
+  </si>
+  <si>
+    <t>0.95-positive</t>
+  </si>
+  <si>
+    <t>own</t>
+  </si>
+  <si>
+    <t>its</t>
+  </si>
+  <si>
+    <t>has</t>
+  </si>
+  <si>
+    <t>goals</t>
+  </si>
+  <si>
+    <t>tool</t>
+  </si>
+  <si>
+    <t>means</t>
+  </si>
+  <si>
+    <t>waiting</t>
+  </si>
+  <si>
+    <t>isn</t>
+  </si>
+  <si>
+    <t>more</t>
+  </si>
+  <si>
+    <t>pursuing</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>of</t>
   </si>
   <si>
     <t>'</t>
   </si>
   <si>
-    <t>and</t>
-  </si>
-  <si>
-    <t>are</t>
-  </si>
-  <si>
-    <t>.</t>
-  </si>
-  <si>
-    <t>the</t>
-  </si>
-  <si>
-    <t>0.95-positive</t>
-  </si>
-  <si>
-    <t>own</t>
-  </si>
-  <si>
-    <t>its</t>
-  </si>
-  <si>
-    <t>goals</t>
-  </si>
-  <si>
-    <t>waiting</t>
-  </si>
-  <si>
-    <t>tool</t>
-  </si>
-  <si>
-    <t>has</t>
-  </si>
-  <si>
-    <t>pursuing</t>
-  </si>
-  <si>
-    <t>means</t>
-  </si>
-  <si>
-    <t>more</t>
-  </si>
-  <si>
-    <t>be</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>"</t>
-  </si>
-  <si>
     <t>social</t>
   </si>
   <si>
-    <t>media</t>
-  </si>
-  <si>
-    <t>of</t>
-  </si>
-  <si>
-    <t>’</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
-    <t>it</t>
-  </si>
-  <si>
-    <t>to</t>
+    <t>…</t>
   </si>
   <si>
     <t>0.8-negative</t>
@@ -539,7 +524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BS23"/>
+  <dimension ref="A1:BS22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -550,25 +535,25 @@
         <v>0</v>
       </c>
       <c r="J1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="S1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BL1" t="s">
         <v>50</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:71">
@@ -770,13 +755,13 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0.1089933698943932</v>
+        <v>0.1431768952033691</v>
       </c>
       <c r="C3">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D3">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -788,19 +773,19 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="K3">
-        <v>0.1107059757098089</v>
+        <v>0.08045334362869733</v>
       </c>
       <c r="L3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -812,19 +797,19 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="T3">
-        <v>0.07369571528924622</v>
+        <v>0.09792878268119339</v>
       </c>
       <c r="U3">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="V3">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="W3">
         <v>1</v>
@@ -836,19 +821,19 @@
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="AC3">
-        <v>0.08595744335700072</v>
+        <v>0.06583217233146796</v>
       </c>
       <c r="AD3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF3">
         <v>0</v>
@@ -860,19 +845,19 @@
         <v>0</v>
       </c>
       <c r="AI3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AK3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AL3">
-        <v>0.06592801777940464</v>
+        <v>0.08722980094359058</v>
       </c>
       <c r="AM3">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AN3">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AO3">
         <v>1</v>
@@ -884,19 +869,19 @@
         <v>0</v>
       </c>
       <c r="AR3">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="AU3">
-        <v>0.08156378826824513</v>
+        <v>0.06370539080885512</v>
       </c>
       <c r="AV3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AW3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AX3">
         <v>0</v>
@@ -908,19 +893,19 @@
         <v>0</v>
       </c>
       <c r="BA3">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="BC3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="BD3">
-        <v>0.0625189199906432</v>
+        <v>0.0824429223283125</v>
       </c>
       <c r="BE3">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="BF3">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="BG3">
         <v>1</v>
@@ -932,19 +917,19 @@
         <v>0</v>
       </c>
       <c r="BJ3">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="BL3" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="BM3">
-        <v>0.07973075805405735</v>
+        <v>0.06285196423286321</v>
       </c>
       <c r="BN3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BO3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BP3">
         <v>0</v>
@@ -956,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="BS3">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:71">
@@ -964,13 +949,13 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.1089851297714834</v>
+        <v>0.1431490884520281</v>
       </c>
       <c r="C4">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -982,13 +967,13 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K4">
-        <v>0.1093986630980081</v>
+        <v>0.07295601265185409</v>
       </c>
       <c r="L4">
         <v>4</v>
@@ -1012,13 +997,13 @@
         <v>10</v>
       </c>
       <c r="T4">
-        <v>0.07368382512157051</v>
+        <v>0.09788624193033367</v>
       </c>
       <c r="U4">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="V4">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="W4">
         <v>1</v>
@@ -1030,13 +1015,13 @@
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="AC4">
-        <v>0.08438065555520634</v>
+        <v>0.06351576825186199</v>
       </c>
       <c r="AD4">
         <v>4</v>
@@ -1060,13 +1045,13 @@
         <v>10</v>
       </c>
       <c r="AL4">
-        <v>0.06591532437298812</v>
+        <v>0.08718377631720574</v>
       </c>
       <c r="AM4">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AN4">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="AO4">
         <v>1</v>
@@ -1078,19 +1063,19 @@
         <v>0</v>
       </c>
       <c r="AR4">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AU4">
-        <v>0.0799391600117955</v>
+        <v>0.06234282561266193</v>
       </c>
       <c r="AV4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AW4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AX4">
         <v>0</v>
@@ -1102,19 +1087,19 @@
         <v>0</v>
       </c>
       <c r="BA4">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="BC4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="BD4">
-        <v>0.06250587405770107</v>
+        <v>0.08239533896581068</v>
       </c>
       <c r="BE4">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="BF4">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="BG4">
         <v>1</v>
@@ -1126,19 +1111,19 @@
         <v>0</v>
       </c>
       <c r="BJ4">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="BL4" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="BM4">
-        <v>0.07808617078920307</v>
+        <v>0.06209581948995218</v>
       </c>
       <c r="BN4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BO4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BP4">
         <v>0</v>
@@ -1150,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="BS4">
-        <v>57</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:71">
@@ -1158,13 +1143,13 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.1089686495256637</v>
+        <v>0.1211307899008824</v>
       </c>
       <c r="C5">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1176,19 +1161,19 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="K5">
-        <v>0.07728342591222714</v>
+        <v>0.07178726248841083</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1200,19 +1185,19 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="T5">
-        <v>0.07366004478621908</v>
+        <v>0.08943304560281211</v>
       </c>
       <c r="U5">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="V5">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="W5">
         <v>1</v>
@@ -1224,19 +1209,19 @@
         <v>0</v>
       </c>
       <c r="Z5">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="AC5">
-        <v>0.07735770432998179</v>
+        <v>0.06295837716979596</v>
       </c>
       <c r="AD5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF5">
         <v>0</v>
@@ -1248,19 +1233,19 @@
         <v>0</v>
       </c>
       <c r="AI5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AL5">
-        <v>0.06588993756015508</v>
+        <v>0.08193806805646578</v>
       </c>
       <c r="AM5">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AN5">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AO5">
         <v>1</v>
@@ -1272,19 +1257,19 @@
         <v>0</v>
       </c>
       <c r="AR5">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AU5">
-        <v>0.07737089112197008</v>
+        <v>0.06221059928739839</v>
       </c>
       <c r="AV5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AW5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AX5">
         <v>0</v>
@@ -1296,19 +1281,19 @@
         <v>0</v>
       </c>
       <c r="BA5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="BC5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="BD5">
-        <v>0.0624797821918168</v>
+        <v>0.07858470709011338</v>
       </c>
       <c r="BE5">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="BF5">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="BG5">
         <v>1</v>
@@ -1320,19 +1305,19 @@
         <v>0</v>
       </c>
       <c r="BJ5">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="BL5" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="BM5">
-        <v>0.07737639264351752</v>
+        <v>0.06196347264123488</v>
       </c>
       <c r="BN5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BO5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BP5">
         <v>0</v>
@@ -1344,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="BS5">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:71">
@@ -1352,13 +1337,13 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.08362161006635534</v>
+        <v>0.08218745994207571</v>
       </c>
       <c r="C6">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1370,19 +1355,19 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="K6">
-        <v>0.0772289545534021</v>
+        <v>0.06719016339863049</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1394,19 +1379,19 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="T6">
-        <v>0.06494439986819159</v>
+        <v>0.07527230283459463</v>
       </c>
       <c r="U6">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="V6">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="W6">
         <v>1</v>
@@ -1418,19 +1403,19 @@
         <v>0</v>
       </c>
       <c r="Z6">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AC6">
-        <v>0.07729200483824036</v>
+        <v>0.06282645119498045</v>
       </c>
       <c r="AD6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF6">
         <v>0</v>
@@ -1442,19 +1427,19 @@
         <v>0</v>
       </c>
       <c r="AI6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AK6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="AL6">
-        <v>0.06083424238690927</v>
+        <v>0.07363720392147786</v>
       </c>
       <c r="AM6">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="AN6">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="AO6">
         <v>1</v>
@@ -1466,19 +1451,19 @@
         <v>0</v>
       </c>
       <c r="AR6">
+        <v>37</v>
+      </c>
+      <c r="AT6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AT6" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="AU6">
-        <v>0.07730319827795135</v>
+        <v>0.06214259937566825</v>
       </c>
       <c r="AV6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AW6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AX6">
         <v>0</v>
@@ -1490,19 +1475,19 @@
         <v>0</v>
       </c>
       <c r="BA6">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="BC6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="BD6">
-        <v>0.05903037080679843</v>
+        <v>0.0729056371039036</v>
       </c>
       <c r="BE6">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="BF6">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="BG6">
         <v>1</v>
@@ -1514,19 +1499,19 @@
         <v>0</v>
       </c>
       <c r="BJ6">
+        <v>37</v>
+      </c>
+      <c r="BL6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="BL6" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="BM6">
-        <v>0.0773078681741486</v>
+        <v>0.06159157953662575</v>
       </c>
       <c r="BN6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BO6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BP6">
         <v>0</v>
@@ -1538,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="BS6">
-        <v>4</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:71">
@@ -1546,13 +1531,13 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.07533027197788181</v>
+        <v>0.07336345647081287</v>
       </c>
       <c r="C7">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D7">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1564,19 +1549,19 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K7">
-        <v>0.07695659775927695</v>
+        <v>0.06706030226935901</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -1588,19 +1573,19 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="T7">
-        <v>0.06133806640862913</v>
+        <v>0.07186549985307017</v>
       </c>
       <c r="U7">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="V7">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="W7">
         <v>1</v>
@@ -1612,19 +1597,19 @@
         <v>0</v>
       </c>
       <c r="Z7">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="AC7">
-        <v>0.0769635073795332</v>
+        <v>0.06232843447852252</v>
       </c>
       <c r="AD7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AE7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AF7">
         <v>0</v>
@@ -1636,19 +1621,19 @@
         <v>0</v>
       </c>
       <c r="AI7">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="AK7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="AL7">
-        <v>0.05825890373979767</v>
+        <v>0.07151130584135099</v>
       </c>
       <c r="AM7">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AN7">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AO7">
         <v>1</v>
@@ -1660,13 +1645,13 @@
         <v>0</v>
       </c>
       <c r="AR7">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="AT7" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AU7">
-        <v>0.07696473405785767</v>
+        <v>0.06135301492228374</v>
       </c>
       <c r="AV7">
         <v>2</v>
@@ -1684,19 +1669,19 @@
         <v>0</v>
       </c>
       <c r="BA7">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="BC7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="BD7">
-        <v>0.05690751658391906</v>
+        <v>0.07135283433612361</v>
       </c>
       <c r="BE7">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="BF7">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="BG7">
         <v>1</v>
@@ -1708,13 +1693,13 @@
         <v>0</v>
       </c>
       <c r="BJ7">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="BL7" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="BM7">
-        <v>0.07696524582730396</v>
+        <v>0.06140893780482298</v>
       </c>
       <c r="BN7">
         <v>2</v>
@@ -1732,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="BS7">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:71">
@@ -1740,13 +1725,13 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.06037914013708395</v>
+        <v>0.06821457582464625</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1758,13 +1743,13 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K8">
-        <v>0.07129157644147356</v>
+        <v>0.06025556398196363</v>
       </c>
       <c r="L8">
         <v>2</v>
@@ -1782,19 +1767,19 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="T8">
-        <v>0.05647965268929479</v>
+        <v>0.06903476846452505</v>
       </c>
       <c r="U8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="V8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="W8">
         <v>1</v>
@@ -1806,19 +1791,19 @@
         <v>0</v>
       </c>
       <c r="Z8">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AC8">
-        <v>0.07226944091557515</v>
+        <v>0.06121365231439048</v>
       </c>
       <c r="AD8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF8">
         <v>0</v>
@@ -1830,19 +1815,19 @@
         <v>0</v>
       </c>
       <c r="AI8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="AL8">
-        <v>0.05562152091604564</v>
+        <v>0.06922870420208933</v>
       </c>
       <c r="AM8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AN8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AO8">
         <v>1</v>
@@ -1854,19 +1839,19 @@
         <v>0</v>
       </c>
       <c r="AR8">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="AT8" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="AU8">
-        <v>0.07446212842060775</v>
+        <v>0.06128690175965196</v>
       </c>
       <c r="AV8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AX8">
         <v>0</v>
@@ -1878,19 +1863,19 @@
         <v>0</v>
       </c>
       <c r="BA8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BC8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="BD8">
-        <v>0.05524490286070258</v>
+        <v>0.06931547384593513</v>
       </c>
       <c r="BE8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="BF8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="BG8">
         <v>1</v>
@@ -1902,19 +1887,19 @@
         <v>0</v>
       </c>
       <c r="BJ8">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="BL8" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="BM8">
-        <v>0.07537691630582047</v>
+        <v>0.06134276438046433</v>
       </c>
       <c r="BN8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BO8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BP8">
         <v>0</v>
@@ -1926,7 +1911,7 @@
         <v>0</v>
       </c>
       <c r="BS8">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:71">
@@ -1934,13 +1919,13 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>0.05735991696405426</v>
+        <v>0.06362183020529864</v>
       </c>
       <c r="C9">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D9">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1952,19 +1937,19 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="K9">
-        <v>0.0599184947075359</v>
+        <v>0.06019063341732788</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1976,19 +1961,19 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="T9">
-        <v>0.05490894633816029</v>
+        <v>0.06705485209317458</v>
       </c>
       <c r="U9">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="V9">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="W9">
         <v>1</v>
@@ -2000,19 +1985,19 @@
         <v>0</v>
       </c>
       <c r="Z9">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="AC9">
-        <v>0.07213804193209228</v>
+        <v>0.06114768932698272</v>
       </c>
       <c r="AD9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF9">
         <v>0</v>
@@ -2024,19 +2009,19 @@
         <v>0</v>
       </c>
       <c r="AI9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AK9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="AL9">
-        <v>0.05436957910142962</v>
+        <v>0.06786659509052444</v>
       </c>
       <c r="AM9">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AN9">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AO9">
         <v>1</v>
@@ -2048,19 +2033,19 @@
         <v>0</v>
       </c>
       <c r="AR9">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="AT9" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="AU9">
-        <v>0.07432674273257028</v>
+        <v>0.06108856227175665</v>
       </c>
       <c r="AV9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AX9">
         <v>0</v>
@@ -2072,19 +2057,19 @@
         <v>0</v>
       </c>
       <c r="BA9">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="BC9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="BD9">
-        <v>0.05413286086520335</v>
+        <v>0.06822978060578323</v>
       </c>
       <c r="BE9">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="BF9">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="BG9">
         <v>1</v>
@@ -2096,19 +2081,19 @@
         <v>0</v>
       </c>
       <c r="BJ9">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="BL9" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="BM9">
-        <v>0.07523986736708263</v>
+        <v>0.06114424410738839</v>
       </c>
       <c r="BN9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BO9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BP9">
         <v>0</v>
@@ -2120,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="BS9">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:71">
@@ -2128,13 +2113,13 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>0.0392906804753086</v>
+        <v>0.0461684705221596</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2146,19 +2131,19 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="K10">
-        <v>0.05980955198988583</v>
+        <v>0.05999584172342068</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -2170,19 +2155,19 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="T10">
-        <v>0.04833714425558294</v>
+        <v>0.06053903138614376</v>
       </c>
       <c r="U10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W10">
         <v>1</v>
@@ -2194,13 +2179,13 @@
         <v>0</v>
       </c>
       <c r="Z10">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AC10">
-        <v>0.07013076023842427</v>
+        <v>0.06094980036475948</v>
       </c>
       <c r="AD10">
         <v>2</v>
@@ -2218,44 +2203,44 @@
         <v>0</v>
       </c>
       <c r="AI10">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="AK10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AL10">
-        <v>0.05032793358606333</v>
+        <v>0.06393697131496455</v>
       </c>
       <c r="AM10">
+        <v>3</v>
+      </c>
+      <c r="AN10">
+        <v>3</v>
+      </c>
+      <c r="AO10">
+        <v>1</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>97</v>
+      </c>
+      <c r="AT10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AU10">
+        <v>0.06095256244829637</v>
+      </c>
+      <c r="AV10">
         <v>4</v>
       </c>
-      <c r="AN10">
+      <c r="AW10">
         <v>4</v>
       </c>
-      <c r="AO10">
-        <v>1</v>
-      </c>
-      <c r="AP10">
-        <v>0</v>
-      </c>
-      <c r="AQ10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR10">
-        <v>96</v>
-      </c>
-      <c r="AT10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU10">
-        <v>0.06992467827990931</v>
-      </c>
-      <c r="AV10">
-        <v>2</v>
-      </c>
-      <c r="AW10">
-        <v>2</v>
-      </c>
       <c r="AX10">
         <v>0</v>
       </c>
@@ -2266,19 +2251,19 @@
         <v>0</v>
       </c>
       <c r="BA10">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="BC10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BD10">
-        <v>0.05144325128624663</v>
+        <v>0.06599812379003646</v>
       </c>
       <c r="BE10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BF10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG10">
         <v>1</v>
@@ -2290,19 +2275,19 @@
         <v>0</v>
       </c>
       <c r="BJ10">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="BL10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BM10">
-        <v>0.06983870101293548</v>
+        <v>0.06072205611969378</v>
       </c>
       <c r="BN10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BO10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BP10">
         <v>0</v>
@@ -2314,7 +2299,7 @@
         <v>0</v>
       </c>
       <c r="BS10">
-        <v>113</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:71">
@@ -2322,13 +2307,13 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>0.03480961735920982</v>
+        <v>0.04458348569572541</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -2340,19 +2325,19 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>15</v>
+        <v>211</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K11">
-        <v>0.05479818697798283</v>
+        <v>0.05826435999980104</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -2364,19 +2349,19 @@
         <v>0</v>
       </c>
       <c r="Q11">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T11">
-        <v>0.04744297324402312</v>
+        <v>0.05900402144244748</v>
       </c>
       <c r="U11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W11">
         <v>1</v>
@@ -2388,13 +2373,13 @@
         <v>0</v>
       </c>
       <c r="Z11">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="AC11">
-        <v>0.06609368869188054</v>
+        <v>0.05946892745898497</v>
       </c>
       <c r="AD11">
         <v>1</v>
@@ -2412,19 +2397,19 @@
         <v>0</v>
       </c>
       <c r="AI11">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="AK11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AL11">
-        <v>0.05022310376955375</v>
+        <v>0.06383615679577054</v>
       </c>
       <c r="AM11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AO11">
         <v>1</v>
@@ -2436,13 +2421,13 @@
         <v>0</v>
       </c>
       <c r="AR11">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AT11" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="AU11">
-        <v>0.06809900108284672</v>
+        <v>0.06036320423190554</v>
       </c>
       <c r="AV11">
         <v>1</v>
@@ -2460,44 +2445,44 @@
         <v>0</v>
       </c>
       <c r="BA11">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="BC11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="BD11">
-        <v>0.05120165395118204</v>
+        <v>0.065457258607736</v>
       </c>
       <c r="BE11">
+        <v>3</v>
+      </c>
+      <c r="BF11">
+        <v>3</v>
+      </c>
+      <c r="BG11">
+        <v>1</v>
+      </c>
+      <c r="BH11">
+        <v>0</v>
+      </c>
+      <c r="BI11" t="b">
+        <v>0</v>
+      </c>
+      <c r="BJ11">
+        <v>97</v>
+      </c>
+      <c r="BL11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="BM11">
+        <v>0.06040045789817013</v>
+      </c>
+      <c r="BN11">
         <v>4</v>
       </c>
-      <c r="BF11">
+      <c r="BO11">
         <v>4</v>
       </c>
-      <c r="BG11">
-        <v>1</v>
-      </c>
-      <c r="BH11">
-        <v>0</v>
-      </c>
-      <c r="BI11" t="b">
-        <v>0</v>
-      </c>
-      <c r="BJ11">
-        <v>96</v>
-      </c>
-      <c r="BL11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="BM11">
-        <v>0.06893561618514127</v>
-      </c>
-      <c r="BN11">
-        <v>1</v>
-      </c>
-      <c r="BO11">
-        <v>1</v>
-      </c>
       <c r="BP11">
         <v>0</v>
       </c>
@@ -2508,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="BS11">
-        <v>94</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:71">
@@ -2516,13 +2501,13 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>0.03391968408494662</v>
+        <v>0.03856796410989857</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -2534,163 +2519,163 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12">
+        <v>0.05332096456529676</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T12">
+        <v>0.05838718055498138</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z12">
         <v>40</v>
       </c>
-      <c r="K12">
-        <v>0.04918763701900446</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>197</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T12">
-        <v>0.0465618966180798</v>
-      </c>
-      <c r="U12">
-        <v>1</v>
-      </c>
-      <c r="V12">
-        <v>1</v>
-      </c>
-      <c r="W12">
-        <v>1</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-      <c r="Y12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z12">
-        <v>11</v>
-      </c>
       <c r="AB12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC12">
+        <v>0.05919078736721952</v>
+      </c>
+      <c r="AD12">
+        <v>2</v>
+      </c>
+      <c r="AE12">
+        <v>2</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>1</v>
+      </c>
+      <c r="AH12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>93</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL12">
+        <v>0.06316879971319039</v>
+      </c>
+      <c r="AM12">
+        <v>1</v>
+      </c>
+      <c r="AN12">
+        <v>1</v>
+      </c>
+      <c r="AO12">
+        <v>1</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR12">
         <v>40</v>
       </c>
-      <c r="AC12">
-        <v>0.05932664104251305</v>
-      </c>
-      <c r="AD12">
-        <v>1</v>
-      </c>
-      <c r="AE12">
-        <v>1</v>
-      </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
-      <c r="AG12">
-        <v>1</v>
-      </c>
-      <c r="AH12" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI12">
-        <v>197</v>
-      </c>
-      <c r="AK12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL12">
-        <v>0.04970737952709595</v>
-      </c>
-      <c r="AM12">
-        <v>1</v>
-      </c>
-      <c r="AN12">
-        <v>1</v>
-      </c>
-      <c r="AO12">
-        <v>1</v>
-      </c>
-      <c r="AP12">
-        <v>0</v>
-      </c>
-      <c r="AQ12" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR12">
-        <v>11</v>
-      </c>
       <c r="AT12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU12">
+        <v>0.05932554460157608</v>
+      </c>
+      <c r="AV12">
+        <v>2</v>
+      </c>
+      <c r="AW12">
+        <v>2</v>
+      </c>
+      <c r="AX12">
+        <v>0</v>
+      </c>
+      <c r="AY12">
+        <v>1</v>
+      </c>
+      <c r="AZ12" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA12">
+        <v>93</v>
+      </c>
+      <c r="BC12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD12">
+        <v>0.06530816503375994</v>
+      </c>
+      <c r="BE12">
+        <v>1</v>
+      </c>
+      <c r="BF12">
+        <v>1</v>
+      </c>
+      <c r="BG12">
+        <v>1</v>
+      </c>
+      <c r="BH12">
+        <v>0</v>
+      </c>
+      <c r="BI12" t="b">
+        <v>0</v>
+      </c>
+      <c r="BJ12">
         <v>40</v>
       </c>
-      <c r="AU12">
-        <v>0.06112663814891709</v>
-      </c>
-      <c r="AV12">
-        <v>1</v>
-      </c>
-      <c r="AW12">
-        <v>1</v>
-      </c>
-      <c r="AX12">
-        <v>0</v>
-      </c>
-      <c r="AY12">
-        <v>1</v>
-      </c>
-      <c r="AZ12" t="b">
-        <v>0</v>
-      </c>
-      <c r="BA12">
-        <v>197</v>
-      </c>
-      <c r="BC12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="BD12">
-        <v>0.05108787340139109</v>
-      </c>
-      <c r="BE12">
-        <v>1</v>
-      </c>
-      <c r="BF12">
-        <v>1</v>
-      </c>
-      <c r="BG12">
-        <v>1</v>
-      </c>
-      <c r="BH12">
-        <v>0</v>
-      </c>
-      <c r="BI12" t="b">
-        <v>0</v>
-      </c>
-      <c r="BJ12">
-        <v>11</v>
-      </c>
       <c r="BL12" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="BM12">
-        <v>0.06187759584014172</v>
+        <v>0.05937961945782451</v>
       </c>
       <c r="BN12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BO12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BP12">
         <v>0</v>
@@ -2702,7 +2687,7 @@
         <v>0</v>
       </c>
       <c r="BS12">
-        <v>197</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:71">
@@ -2710,13 +2695,13 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>0.03318631314597045</v>
+        <v>0.03816476621545478</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -2728,19 +2713,19 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>212</v>
+        <v>40</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K13">
-        <v>0.04443719654073246</v>
+        <v>0.05292708270031366</v>
       </c>
       <c r="L13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -2752,19 +2737,19 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>606</v>
+        <v>661</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="T13">
-        <v>0.04621708175548422</v>
+        <v>0.05811420858713907</v>
       </c>
       <c r="U13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W13">
         <v>1</v>
@@ -2776,13 +2761,13 @@
         <v>0</v>
       </c>
       <c r="Z13">
-        <v>40</v>
+        <v>211</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AC13">
-        <v>0.04966881575652255</v>
+        <v>0.05421387612883435</v>
       </c>
       <c r="AD13">
         <v>1</v>
@@ -2800,19 +2785,19 @@
         <v>0</v>
       </c>
       <c r="AI13">
-        <v>344</v>
+        <v>239</v>
       </c>
       <c r="AK13" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="AL13">
-        <v>0.04933927074101685</v>
+        <v>0.06131356761102876</v>
       </c>
       <c r="AM13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AN13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AO13">
         <v>1</v>
@@ -2824,13 +2809,13 @@
         <v>0</v>
       </c>
       <c r="AR13">
-        <v>40</v>
+        <v>211</v>
       </c>
       <c r="AT13" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AU13">
-        <v>0.05117579007816314</v>
+        <v>0.05509618894224109</v>
       </c>
       <c r="AV13">
         <v>1</v>
@@ -2848,19 +2833,19 @@
         <v>0</v>
       </c>
       <c r="BA13">
-        <v>344</v>
+        <v>239</v>
       </c>
       <c r="BC13" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="BD13">
-        <v>0.05070954134606925</v>
+        <v>0.06274500694513177</v>
       </c>
       <c r="BE13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BF13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BG13">
         <v>1</v>
@@ -2872,13 +2857,13 @@
         <v>0</v>
       </c>
       <c r="BJ13">
-        <v>40</v>
+        <v>211</v>
       </c>
       <c r="BL13" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="BM13">
-        <v>0.05180449884290934</v>
+        <v>0.05545023997912168</v>
       </c>
       <c r="BN13">
         <v>1</v>
@@ -2896,7 +2881,7 @@
         <v>0</v>
       </c>
       <c r="BS13">
-        <v>344</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:71">
@@ -2904,31 +2889,31 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <v>0.03300836862998048</v>
+        <v>0.03690419067753228</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="G14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>546</v>
+        <v>447</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="K14">
-        <v>0.04118034727172466</v>
+        <v>0.04814816291598308</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -2946,67 +2931,67 @@
         <v>0</v>
       </c>
       <c r="Q14">
+        <v>239</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14">
+        <v>0.05608998000855588</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>148</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC14">
+        <v>0.05190517156956317</v>
+      </c>
+      <c r="AD14">
+        <v>1</v>
+      </c>
+      <c r="AE14">
+        <v>1</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>1</v>
+      </c>
+      <c r="AH14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI14">
         <v>344</v>
       </c>
-      <c r="S14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T14">
-        <v>0.04615883513504646</v>
-      </c>
-      <c r="U14">
-        <v>2</v>
-      </c>
-      <c r="V14">
-        <v>2</v>
-      </c>
-      <c r="W14">
-        <v>1</v>
-      </c>
-      <c r="X14">
-        <v>0</v>
-      </c>
-      <c r="Y14" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z14">
-        <v>123</v>
-      </c>
-      <c r="AB14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC14">
-        <v>0.03774091080989832</v>
-      </c>
-      <c r="AD14">
-        <v>2</v>
-      </c>
-      <c r="AE14">
-        <v>2</v>
-      </c>
-      <c r="AF14">
-        <v>0</v>
-      </c>
-      <c r="AG14">
-        <v>1</v>
-      </c>
-      <c r="AH14" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI14">
-        <v>606</v>
-      </c>
       <c r="AK14" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="AL14">
-        <v>0.04885221587656949</v>
+        <v>0.06068346988840912</v>
       </c>
       <c r="AM14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AO14">
         <v>1</v>
@@ -3018,43 +3003,43 @@
         <v>0</v>
       </c>
       <c r="AR14">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="AT14" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="AU14">
-        <v>0.03750183558637881</v>
+        <v>0.0527822282501291</v>
       </c>
       <c r="AV14">
         <v>1</v>
       </c>
       <c r="AW14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AX14">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="AY14">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="AZ14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA14">
-        <v>546</v>
+        <v>344</v>
       </c>
       <c r="BC14" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="BD14">
-        <v>0.05003429052849631</v>
+        <v>0.06273866345866119</v>
       </c>
       <c r="BE14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BF14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG14">
         <v>1</v>
@@ -3066,31 +3051,31 @@
         <v>0</v>
       </c>
       <c r="BJ14">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="BL14" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="BM14">
-        <v>0.03796255603038595</v>
+        <v>0.0531341701265691</v>
       </c>
       <c r="BN14">
         <v>1</v>
       </c>
       <c r="BO14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="BP14">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="BQ14">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="BR14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS14">
-        <v>546</v>
+        <v>344</v>
       </c>
     </row>
     <row r="15" spans="1:71">
@@ -3098,7 +3083,7 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <v>0.03226832131495112</v>
+        <v>0.03666320164304345</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3116,19 +3101,19 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>11</v>
+        <v>148</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K15">
-        <v>0.03532904735645787</v>
+        <v>0.04587559315373229</v>
       </c>
       <c r="L15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -3140,13 +3125,13 @@
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>1095</v>
+        <v>344</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="T15">
-        <v>0.04510061021190828</v>
+        <v>0.0514122688703584</v>
       </c>
       <c r="U15">
         <v>2</v>
@@ -3164,43 +3149,43 @@
         <v>0</v>
       </c>
       <c r="Z15">
-        <v>212</v>
+        <v>447</v>
       </c>
       <c r="AB15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC15">
+        <v>0.04846850760256057</v>
+      </c>
+      <c r="AD15">
+        <v>3</v>
+      </c>
+      <c r="AE15">
+        <v>3</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>1</v>
+      </c>
+      <c r="AH15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <v>661</v>
+      </c>
+      <c r="AK15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AC15">
-        <v>0.03639751842475329</v>
-      </c>
-      <c r="AD15">
-        <v>1</v>
-      </c>
-      <c r="AE15">
-        <v>4</v>
-      </c>
-      <c r="AF15">
-        <v>0.75</v>
-      </c>
-      <c r="AG15">
-        <v>0.25</v>
-      </c>
-      <c r="AH15" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI15">
-        <v>546</v>
-      </c>
-      <c r="AK15" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="AL15">
-        <v>0.04796838284803259</v>
+        <v>0.05484272497074683</v>
       </c>
       <c r="AM15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO15">
         <v>1</v>
@@ -3212,19 +3197,19 @@
         <v>0</v>
       </c>
       <c r="AR15">
-        <v>148</v>
+        <v>447</v>
       </c>
       <c r="AT15" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AU15">
-        <v>0.03655210617867328</v>
+        <v>0.04781996755454951</v>
       </c>
       <c r="AV15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AW15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AX15">
         <v>0</v>
@@ -3236,19 +3221,19 @@
         <v>0</v>
       </c>
       <c r="BA15">
-        <v>606</v>
+        <v>661</v>
       </c>
       <c r="BC15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="BD15">
-        <v>0.04930058058831892</v>
+        <v>0.05637756046727689</v>
       </c>
       <c r="BE15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BF15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BG15">
         <v>1</v>
@@ -3260,19 +3245,19 @@
         <v>0</v>
       </c>
       <c r="BJ15">
-        <v>148</v>
+        <v>447</v>
       </c>
       <c r="BL15" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="BM15">
-        <v>0.03605613761405411</v>
+        <v>0.04755972393916973</v>
       </c>
       <c r="BN15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BO15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BP15">
         <v>0</v>
@@ -3284,7 +3269,7 @@
         <v>0</v>
       </c>
       <c r="BS15">
-        <v>606</v>
+        <v>661</v>
       </c>
     </row>
     <row r="16" spans="1:71">
@@ -3292,13 +3277,13 @@
         <v>22</v>
       </c>
       <c r="B16">
-        <v>0.03202935775056562</v>
+        <v>0.03301587713788993</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -3310,37 +3295,37 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>40</v>
+        <v>1043</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="K16">
-        <v>0.03017713278906808</v>
+        <v>0.03949942682007313</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N16">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="O16">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="P16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>546</v>
+        <v>960</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="T16">
-        <v>0.04493294364650755</v>
+        <v>0.04756055946117973</v>
       </c>
       <c r="U16">
         <v>1</v>
@@ -3358,13 +3343,13 @@
         <v>0</v>
       </c>
       <c r="Z16">
-        <v>148</v>
+        <v>549</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AC16">
-        <v>0.02871067789100576</v>
+        <v>0.04383569944334862</v>
       </c>
       <c r="AD16">
         <v>1</v>
@@ -3382,19 +3367,19 @@
         <v>0</v>
       </c>
       <c r="AI16">
-        <v>663</v>
+        <v>711</v>
       </c>
       <c r="AK16" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="AL16">
-        <v>0.04772250270549914</v>
+        <v>0.05145553229824908</v>
       </c>
       <c r="AM16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AO16">
         <v>1</v>
@@ -3406,13 +3391,13 @@
         <v>0</v>
       </c>
       <c r="AR16">
-        <v>212</v>
+        <v>549</v>
       </c>
       <c r="AT16" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AU16">
-        <v>0.02958177283618689</v>
+        <v>0.04469438468817575</v>
       </c>
       <c r="AV16">
         <v>1</v>
@@ -3430,19 +3415,19 @@
         <v>0</v>
       </c>
       <c r="BA16">
-        <v>663</v>
+        <v>711</v>
       </c>
       <c r="BC16" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="BD16">
-        <v>0.04887320249664652</v>
+        <v>0.05319819927704453</v>
       </c>
       <c r="BE16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BF16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG16">
         <v>1</v>
@@ -3454,13 +3439,13 @@
         <v>0</v>
       </c>
       <c r="BJ16">
-        <v>212</v>
+        <v>549</v>
       </c>
       <c r="BL16" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="BM16">
-        <v>0.02994519311422141</v>
+        <v>0.04503895454669481</v>
       </c>
       <c r="BN16">
         <v>1</v>
@@ -3478,7 +3463,7 @@
         <v>0</v>
       </c>
       <c r="BS16">
-        <v>663</v>
+        <v>711</v>
       </c>
     </row>
     <row r="17" spans="1:71">
@@ -3486,7 +3471,7 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>0.03113942447630242</v>
+        <v>0.03108794799918285</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -3504,13 +3489,13 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>148</v>
+        <v>549</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="K17">
-        <v>0.02380398380653926</v>
+        <v>0.03793242074662717</v>
       </c>
       <c r="L17">
         <v>1</v>
@@ -3528,19 +3513,19 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>663</v>
+        <v>711</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="T17">
-        <v>0.04446922710715487</v>
+        <v>0.0404172562294908</v>
       </c>
       <c r="U17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W17">
         <v>1</v>
@@ -3552,13 +3537,13 @@
         <v>0</v>
       </c>
       <c r="Z17">
-        <v>187</v>
+        <v>1043</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AC17">
-        <v>0.02555710228741702</v>
+        <v>0.04337395853149439</v>
       </c>
       <c r="AD17">
         <v>1</v>
@@ -3576,19 +3561,19 @@
         <v>0</v>
       </c>
       <c r="AI17">
-        <v>711</v>
+        <v>732</v>
       </c>
       <c r="AK17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="AL17">
-        <v>0.04747333999778827</v>
+        <v>0.04216732303493608</v>
       </c>
       <c r="AM17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AN17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AO17">
         <v>1</v>
@@ -3600,13 +3585,13 @@
         <v>0</v>
       </c>
       <c r="AR17">
-        <v>187</v>
+        <v>1043</v>
       </c>
       <c r="AT17" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AU17">
-        <v>0.02633251632328765</v>
+        <v>0.04423159254975335</v>
       </c>
       <c r="AV17">
         <v>1</v>
@@ -3624,19 +3609,19 @@
         <v>0</v>
       </c>
       <c r="BA17">
-        <v>711</v>
+        <v>732</v>
       </c>
       <c r="BC17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="BD17">
-        <v>0.04879178920357576</v>
+        <v>0.04295032814437101</v>
       </c>
       <c r="BE17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BF17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BG17">
         <v>1</v>
@@ -3648,13 +3633,13 @@
         <v>0</v>
       </c>
       <c r="BJ17">
-        <v>187</v>
+        <v>1043</v>
       </c>
       <c r="BL17" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="BM17">
-        <v>0.02665601858451287</v>
+        <v>0.04457574057618428</v>
       </c>
       <c r="BN17">
         <v>1</v>
@@ -3672,7 +3657,7 @@
         <v>0</v>
       </c>
       <c r="BS17">
-        <v>711</v>
+        <v>732</v>
       </c>
     </row>
     <row r="18" spans="1:71">
@@ -3680,31 +3665,31 @@
         <v>24</v>
       </c>
       <c r="B18">
-        <v>0.03081805968281848</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>0.6699999999999999</v>
       </c>
       <c r="G18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>187</v>
+        <v>2785</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="K18">
-        <v>0.02118935858293769</v>
+        <v>0.03747790679417701</v>
       </c>
       <c r="L18">
         <v>1</v>
@@ -3722,237 +3707,189 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>711</v>
+        <v>732</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="T18">
-        <v>0.04205793150486734</v>
+        <v>0</v>
       </c>
       <c r="U18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W18">
-        <v>0.75</v>
+        <v>0.33</v>
       </c>
       <c r="X18">
-        <v>0.25</v>
+        <v>0.6699999999999999</v>
       </c>
       <c r="Y18" t="b">
         <v>1</v>
       </c>
       <c r="Z18">
-        <v>546</v>
+        <v>2785</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="AC18">
-        <v>0.02430881194432982</v>
+        <v>0.04018574747345321</v>
       </c>
       <c r="AD18">
         <v>1</v>
       </c>
       <c r="AE18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF18">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="AG18">
+        <v>1</v>
+      </c>
+      <c r="AH18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI18">
+        <v>877</v>
+      </c>
+      <c r="AK18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL18">
+        <v>0</v>
+      </c>
+      <c r="AM18">
+        <v>1</v>
+      </c>
+      <c r="AN18">
+        <v>3</v>
+      </c>
+      <c r="AO18">
         <v>0.33</v>
       </c>
-      <c r="AH18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI18">
-        <v>730</v>
-      </c>
-      <c r="AK18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL18">
-        <v>0.04416036092307631</v>
-      </c>
-      <c r="AM18">
-        <v>1</v>
-      </c>
-      <c r="AN18">
-        <v>1</v>
-      </c>
-      <c r="AO18">
-        <v>1</v>
-      </c>
       <c r="AP18">
-        <v>0</v>
+        <v>0.6699999999999999</v>
       </c>
       <c r="AQ18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR18">
-        <v>448</v>
+        <v>2785</v>
       </c>
       <c r="AT18" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="AU18">
-        <v>0.02504635228693169</v>
+        <v>0.04103612302255107</v>
       </c>
       <c r="AV18">
         <v>1</v>
       </c>
       <c r="AW18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AX18">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="AY18">
+        <v>1</v>
+      </c>
+      <c r="AZ18" t="b">
+        <v>0</v>
+      </c>
+      <c r="BA18">
+        <v>877</v>
+      </c>
+      <c r="BC18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BD18">
+        <v>0</v>
+      </c>
+      <c r="BE18">
+        <v>1</v>
+      </c>
+      <c r="BF18">
+        <v>3</v>
+      </c>
+      <c r="BG18">
         <v>0.33</v>
       </c>
-      <c r="AZ18" t="b">
-        <v>1</v>
-      </c>
-      <c r="BA18">
-        <v>730</v>
-      </c>
-      <c r="BC18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="BD18">
-        <v>0.04538680070567916</v>
-      </c>
-      <c r="BE18">
-        <v>1</v>
-      </c>
-      <c r="BF18">
-        <v>1</v>
-      </c>
-      <c r="BG18">
-        <v>1</v>
-      </c>
       <c r="BH18">
-        <v>0</v>
+        <v>0.6699999999999999</v>
       </c>
       <c r="BI18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ18">
-        <v>448</v>
+        <v>2785</v>
       </c>
       <c r="BL18" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="BM18">
-        <v>0.02535405366650325</v>
+        <v>0.04137735839884976</v>
       </c>
       <c r="BN18">
         <v>1</v>
       </c>
       <c r="BO18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BP18">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="BQ18">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="BR18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS18">
-        <v>730</v>
+        <v>877</v>
       </c>
     </row>
     <row r="19" spans="1:71">
-      <c r="A19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19">
-        <v>0.028917929478671</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-      <c r="E19">
-        <v>0.67</v>
-      </c>
-      <c r="F19">
-        <v>0.33</v>
-      </c>
-      <c r="G19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>730</v>
-      </c>
       <c r="J19" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="K19">
-        <v>0.02015440276526207</v>
+        <v>0.03655590788991974</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N19">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="O19">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="P19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q19">
-        <v>730</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="T19">
-        <v>0.0413658933437946</v>
-      </c>
-      <c r="U19">
-        <v>1</v>
-      </c>
-      <c r="V19">
-        <v>1</v>
-      </c>
-      <c r="W19">
-        <v>1</v>
-      </c>
-      <c r="X19">
-        <v>0</v>
-      </c>
-      <c r="Y19" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z19">
-        <v>448</v>
+        <v>1096</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AC19">
-        <v>0.02102383735725822</v>
+        <v>0.04012748400638025</v>
       </c>
       <c r="AD19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF19">
         <v>0</v>
@@ -3964,43 +3901,19 @@
         <v>0</v>
       </c>
       <c r="AI19">
-        <v>780</v>
-      </c>
-      <c r="AK19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL19">
-        <v>0.04404940283050503</v>
-      </c>
-      <c r="AM19">
-        <v>3</v>
-      </c>
-      <c r="AN19">
-        <v>4</v>
-      </c>
-      <c r="AO19">
-        <v>0.75</v>
-      </c>
-      <c r="AP19">
-        <v>0.25</v>
-      </c>
-      <c r="AQ19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AR19">
-        <v>546</v>
+        <v>960</v>
       </c>
       <c r="AT19" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AU19">
-        <v>0.02166171008599498</v>
+        <v>0.04021884060099418</v>
       </c>
       <c r="AV19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AX19">
         <v>0</v>
@@ -4012,43 +3925,19 @@
         <v>0</v>
       </c>
       <c r="BA19">
-        <v>780</v>
-      </c>
-      <c r="BC19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="BD19">
-        <v>0.04492342251059832</v>
-      </c>
-      <c r="BE19">
-        <v>3</v>
-      </c>
-      <c r="BF19">
-        <v>4</v>
-      </c>
-      <c r="BG19">
-        <v>0.75</v>
-      </c>
-      <c r="BH19">
-        <v>0.25</v>
-      </c>
-      <c r="BI19" t="b">
-        <v>1</v>
-      </c>
-      <c r="BJ19">
-        <v>546</v>
+        <v>960</v>
       </c>
       <c r="BL19" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="BM19">
-        <v>0.02192783019805686</v>
+        <v>0.04025549981817598</v>
       </c>
       <c r="BN19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BO19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BP19">
         <v>0</v>
@@ -4060,39 +3949,15 @@
         <v>0</v>
       </c>
       <c r="BS19">
-        <v>780</v>
+        <v>960</v>
       </c>
     </row>
     <row r="20" spans="1:71">
-      <c r="A20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20">
-        <v>0.02891302754378775</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>1043</v>
-      </c>
       <c r="J20" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K20">
-        <v>0.01743083482401044</v>
+        <v>0.03433959617011641</v>
       </c>
       <c r="L20">
         <v>1</v>
@@ -4110,43 +3975,19 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>780</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T20">
-        <v>0.03894150335589058</v>
-      </c>
-      <c r="U20">
-        <v>2</v>
-      </c>
-      <c r="V20">
-        <v>3</v>
-      </c>
-      <c r="W20">
-        <v>0.67</v>
-      </c>
-      <c r="X20">
-        <v>0.33</v>
-      </c>
-      <c r="Y20" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z20">
-        <v>730</v>
+        <v>877</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="AC20">
-        <v>0.01465098665833932</v>
+        <v>0.03713716191056232</v>
       </c>
       <c r="AD20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF20">
         <v>0</v>
@@ -4158,43 +3999,19 @@
         <v>0</v>
       </c>
       <c r="AI20">
-        <v>877</v>
-      </c>
-      <c r="AK20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AL20">
-        <v>0.0411473181817413</v>
-      </c>
-      <c r="AM20">
-        <v>2</v>
-      </c>
-      <c r="AN20">
-        <v>3</v>
-      </c>
-      <c r="AO20">
-        <v>0.67</v>
-      </c>
-      <c r="AP20">
-        <v>0.33</v>
-      </c>
-      <c r="AQ20" t="b">
-        <v>1</v>
-      </c>
-      <c r="AR20">
-        <v>730</v>
+        <v>1096</v>
       </c>
       <c r="AT20" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="AU20">
-        <v>0.01509550421617775</v>
+        <v>0.03722171056168722</v>
       </c>
       <c r="AV20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AX20">
         <v>0</v>
@@ -4206,43 +4023,19 @@
         <v>0</v>
       </c>
       <c r="BA20">
-        <v>877</v>
-      </c>
-      <c r="BC20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="BD20">
-        <v>0.04211540923262186</v>
-      </c>
-      <c r="BE20">
-        <v>2</v>
-      </c>
-      <c r="BF20">
-        <v>3</v>
-      </c>
-      <c r="BG20">
-        <v>0.67</v>
-      </c>
-      <c r="BH20">
-        <v>0.33</v>
-      </c>
-      <c r="BI20" t="b">
-        <v>1</v>
-      </c>
-      <c r="BJ20">
-        <v>730</v>
+        <v>1096</v>
       </c>
       <c r="BL20" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="BM20">
-        <v>0.01528095666927087</v>
+        <v>0.03725563791391739</v>
       </c>
       <c r="BN20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BO20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BP20">
         <v>0</v>
@@ -4254,39 +4047,15 @@
         <v>0</v>
       </c>
       <c r="BS20">
-        <v>877</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="21" spans="1:71">
-      <c r="A21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21">
-        <v>0.02866738760334907</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>448</v>
-      </c>
       <c r="J21" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K21">
-        <v>0.01214711301798228</v>
+        <v>0.01576945468429573</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -4304,43 +4073,19 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>877</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T21">
-        <v>0.03614851817003955</v>
-      </c>
-      <c r="U21">
-        <v>3</v>
-      </c>
-      <c r="V21">
-        <v>3</v>
-      </c>
-      <c r="W21">
-        <v>1</v>
-      </c>
-      <c r="X21">
-        <v>0</v>
-      </c>
-      <c r="Y21" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z21">
-        <v>1043</v>
+        <v>1735</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AC21">
-        <v>0.01089922123796904</v>
+        <v>0.02132033307483719</v>
       </c>
       <c r="AD21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AE21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF21">
         <v>0</v>
@@ -4352,37 +4097,13 @@
         <v>0</v>
       </c>
       <c r="AI21">
-        <v>1095</v>
-      </c>
-      <c r="AK21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL21">
-        <v>0.03774077984149413</v>
-      </c>
-      <c r="AM21">
-        <v>3</v>
-      </c>
-      <c r="AN21">
-        <v>3</v>
-      </c>
-      <c r="AO21">
-        <v>1</v>
-      </c>
-      <c r="AP21">
-        <v>0</v>
-      </c>
-      <c r="AQ21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR21">
-        <v>1043</v>
+        <v>1735</v>
       </c>
       <c r="AT21" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="AU21">
-        <v>0.009409305318604068</v>
+        <v>0.02212775850986449</v>
       </c>
       <c r="AV21">
         <v>1</v>
@@ -4400,37 +4121,13 @@
         <v>0</v>
       </c>
       <c r="BA21">
-        <v>961</v>
-      </c>
-      <c r="BC21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="BD21">
-        <v>0.03843959383835844</v>
-      </c>
-      <c r="BE21">
-        <v>3</v>
-      </c>
-      <c r="BF21">
-        <v>3</v>
-      </c>
-      <c r="BG21">
-        <v>1</v>
-      </c>
-      <c r="BH21">
-        <v>0</v>
-      </c>
-      <c r="BI21" t="b">
-        <v>0</v>
-      </c>
-      <c r="BJ21">
-        <v>1043</v>
+        <v>1735</v>
       </c>
       <c r="BL21" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="BM21">
-        <v>0.009524901242280953</v>
+        <v>0.02245175903227716</v>
       </c>
       <c r="BN21">
         <v>1</v>
@@ -4448,395 +4145,105 @@
         <v>0</v>
       </c>
       <c r="BS21">
-        <v>961</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="22" spans="1:71">
-      <c r="A22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22">
-        <v>0.009393740117222752</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>2787</v>
-      </c>
       <c r="J22" s="1" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="K22">
-        <v>0.00757151887667954</v>
+        <v>0</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N22">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="O22">
-        <v>1</v>
+        <v>0.6699999999999999</v>
       </c>
       <c r="P22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22">
-        <v>961</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="T22">
-        <v>0.01355479115030924</v>
-      </c>
-      <c r="U22">
-        <v>1</v>
-      </c>
-      <c r="V22">
-        <v>1</v>
-      </c>
-      <c r="W22">
-        <v>1</v>
-      </c>
-      <c r="X22">
-        <v>0</v>
-      </c>
-      <c r="Y22" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z22">
-        <v>2787</v>
+        <v>2785</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="AC22">
-        <v>0.009132229352059045</v>
+        <v>0</v>
       </c>
       <c r="AD22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AF22">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="AG22">
-        <v>1</v>
+        <v>0.6699999999999999</v>
       </c>
       <c r="AH22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI22">
-        <v>961</v>
-      </c>
-      <c r="AK22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL22">
-        <v>0.01447048331483386</v>
-      </c>
-      <c r="AM22">
-        <v>1</v>
-      </c>
-      <c r="AN22">
-        <v>1</v>
-      </c>
-      <c r="AO22">
-        <v>1</v>
-      </c>
-      <c r="AP22">
-        <v>0</v>
-      </c>
-      <c r="AQ22" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR22">
-        <v>2787</v>
+        <v>2785</v>
       </c>
       <c r="AT22" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="AU22">
-        <v>0.006562146686930735</v>
+        <v>0</v>
       </c>
       <c r="AV22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AW22">
         <v>3</v>
       </c>
       <c r="AX22">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="AY22">
-        <v>1</v>
+        <v>0.6699999999999999</v>
       </c>
       <c r="AZ22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA22">
-        <v>1095</v>
-      </c>
-      <c r="BC22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="BD22">
-        <v>0.01487236355403111</v>
-      </c>
-      <c r="BE22">
-        <v>1</v>
-      </c>
-      <c r="BF22">
-        <v>1</v>
-      </c>
-      <c r="BG22">
-        <v>1</v>
-      </c>
-      <c r="BH22">
-        <v>0</v>
-      </c>
-      <c r="BI22" t="b">
-        <v>0</v>
-      </c>
-      <c r="BJ22">
-        <v>2787</v>
+        <v>2785</v>
       </c>
       <c r="BL22" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="BM22">
-        <v>0.004752721838452287</v>
+        <v>0</v>
       </c>
       <c r="BN22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BO22">
         <v>3</v>
       </c>
       <c r="BP22">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="BQ22">
-        <v>1</v>
+        <v>0.6699999999999999</v>
       </c>
       <c r="BR22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS22">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="23" spans="1:71">
-      <c r="A23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>3927</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>1</v>
-      </c>
-      <c r="P23" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>1100</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <v>1</v>
-      </c>
-      <c r="V23">
-        <v>1</v>
-      </c>
-      <c r="W23">
-        <v>1</v>
-      </c>
-      <c r="X23">
-        <v>0</v>
-      </c>
-      <c r="Y23" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z23">
-        <v>3927</v>
-      </c>
-      <c r="AB23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC23">
-        <v>0</v>
-      </c>
-      <c r="AD23">
-        <v>1</v>
-      </c>
-      <c r="AE23">
-        <v>1</v>
-      </c>
-      <c r="AF23">
-        <v>0</v>
-      </c>
-      <c r="AG23">
-        <v>1</v>
-      </c>
-      <c r="AH23" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI23">
-        <v>1100</v>
-      </c>
-      <c r="AK23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AL23">
-        <v>0</v>
-      </c>
-      <c r="AM23">
-        <v>1</v>
-      </c>
-      <c r="AN23">
-        <v>1</v>
-      </c>
-      <c r="AO23">
-        <v>1</v>
-      </c>
-      <c r="AP23">
-        <v>0</v>
-      </c>
-      <c r="AQ23" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR23">
-        <v>3927</v>
-      </c>
-      <c r="AT23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AU23">
-        <v>0</v>
-      </c>
-      <c r="AV23">
-        <v>1</v>
-      </c>
-      <c r="AW23">
-        <v>1</v>
-      </c>
-      <c r="AX23">
-        <v>0</v>
-      </c>
-      <c r="AY23">
-        <v>1</v>
-      </c>
-      <c r="AZ23" t="b">
-        <v>0</v>
-      </c>
-      <c r="BA23">
-        <v>1100</v>
-      </c>
-      <c r="BC23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="BD23">
-        <v>0</v>
-      </c>
-      <c r="BE23">
-        <v>1</v>
-      </c>
-      <c r="BF23">
-        <v>1</v>
-      </c>
-      <c r="BG23">
-        <v>1</v>
-      </c>
-      <c r="BH23">
-        <v>0</v>
-      </c>
-      <c r="BI23" t="b">
-        <v>0</v>
-      </c>
-      <c r="BJ23">
-        <v>3927</v>
-      </c>
-      <c r="BL23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BM23">
-        <v>0</v>
-      </c>
-      <c r="BN23">
-        <v>1</v>
-      </c>
-      <c r="BO23">
-        <v>1</v>
-      </c>
-      <c r="BP23">
-        <v>0</v>
-      </c>
-      <c r="BQ23">
-        <v>1</v>
-      </c>
-      <c r="BR23" t="b">
-        <v>0</v>
-      </c>
-      <c r="BS23">
-        <v>1100</v>
+        <v>2785</v>
       </c>
     </row>
   </sheetData>

</xml_diff>